<commit_message>
fixing key problems in old database sheets
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0647.xlsx
+++ b/bioSample/bioSample_0647.xlsx
@@ -220,7 +220,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -266,7 +266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -274,7 +274,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>14</v>
@@ -295,7 +295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -303,7 +303,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2</v>
+        <v>138</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>14</v>
@@ -324,7 +324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -332,7 +332,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>14</v>
@@ -353,7 +353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
@@ -361,7 +361,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>14</v>
@@ -382,7 +382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
@@ -390,7 +390,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>14</v>
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
@@ -419,7 +419,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6</v>
+        <v>142</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>14</v>
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>12</v>
       </c>
@@ -448,7 +448,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>7</v>
+        <v>143</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>14</v>
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>12</v>
       </c>
@@ -477,7 +477,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>8</v>
+        <v>144</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>14</v>
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>12</v>
       </c>
@@ -506,7 +506,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>9</v>
+        <v>145</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>14</v>
@@ -527,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>22</v>
       </c>
@@ -535,7 +535,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>14</v>
@@ -556,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
@@ -564,7 +564,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>14</v>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>22</v>
       </c>
@@ -593,7 +593,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>14</v>
@@ -614,7 +614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>22</v>
       </c>
@@ -622,7 +622,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>14</v>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
@@ -651,7 +651,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>14</v>
@@ -672,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
@@ -680,7 +680,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>14</v>
@@ -701,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>22</v>
       </c>
@@ -709,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>14</v>
@@ -730,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>22</v>
       </c>
@@ -738,7 +738,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>17</v>
+        <v>153</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>14</v>
@@ -759,7 +759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>22</v>
       </c>
@@ -767,7 +767,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>18</v>
+        <v>154</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>14</v>

</xml_diff>